<commit_message>
Revisi Rekap Kemiskinan Excel GKM & GKNM
</commit_message>
<xml_diff>
--- a/Rekap/RekapKemiskinan.xlsx
+++ b/Rekap/RekapKemiskinan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>No</t>
   </si>
@@ -22,7 +22,13 @@
     <t>Kecamatan</t>
   </si>
   <si>
-    <t>Garis Kemiskinan (Rp)</t>
+    <t>Garis Kemiskinan Makanan</t>
+  </si>
+  <si>
+    <t>Garis Kemiskinan Non Makanan</t>
+  </si>
+  <si>
+    <t>Garis Kemiskinan</t>
   </si>
   <si>
     <t>Persentase Penduduk Miskin %</t>
@@ -123,12 +129,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="&quot;Rp&quot;#,##0_);[Red]\(&quot;Rp&quot;#,##0\)"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="0.00_ "/>
+    <numFmt numFmtId="179" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="0.00_ "/>
-    <numFmt numFmtId="178" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="180" formatCode="&quot;Rp&quot;#,##0_);[Red]\(&quot;Rp&quot;#,##0\)"/>
+    <numFmt numFmtId="180" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -147,6 +153,21 @@
     </font>
     <font>
       <sz val="12"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
@@ -156,19 +177,11 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -178,8 +191,101 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -194,100 +300,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -295,13 +308,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -324,139 +330,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -468,43 +510,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -547,25 +553,31 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -594,32 +606,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -646,150 +652,150 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -803,41 +809,47 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="1" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="1" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="4" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1158,23 +1170,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.42857142857143" style="1" customWidth="1"/>
     <col min="2" max="2" width="26.2857142857143" customWidth="1"/>
-    <col min="3" max="3" width="20.2857142857143" customWidth="1"/>
-    <col min="4" max="5" width="12.5714285714286" customWidth="1"/>
-    <col min="6" max="6" width="12.8571428571429"/>
-    <col min="7" max="7" width="12.9333333333333" customWidth="1"/>
+    <col min="3" max="4" width="18.7142857142857" customWidth="1"/>
+    <col min="5" max="5" width="19.7142857142857" customWidth="1"/>
+    <col min="6" max="9" width="12.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="47.25" customHeight="1" spans="1:7">
+    <row r="1" ht="47.25" customHeight="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1196,604 +1207,766 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" ht="15.75" spans="1:7">
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" ht="15.75" spans="1:9">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2" s="5">
+        <v>177141.8</v>
+      </c>
+      <c r="D2" s="6">
+        <v>144934.2</v>
+      </c>
+      <c r="E2" s="6">
         <v>322076</v>
       </c>
-      <c r="D2" s="6">
+      <c r="F2" s="7">
         <v>10.86</v>
       </c>
-      <c r="E2" s="7">
+      <c r="G2" s="8">
         <v>7.9278</v>
       </c>
-      <c r="F2" s="8">
+      <c r="H2" s="9">
         <v>1.28</v>
       </c>
-      <c r="G2" s="8">
+      <c r="I2" s="9">
         <v>0.33</v>
       </c>
     </row>
-    <row r="3" ht="15.75" spans="1:7">
+    <row r="3" ht="15.75" spans="1:9">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" s="5">
+        <v>200626.8</v>
+      </c>
+      <c r="D3" s="6">
+        <v>164149.2</v>
+      </c>
+      <c r="E3" s="6">
         <v>364776</v>
       </c>
-      <c r="D3" s="6">
+      <c r="F3" s="7">
         <v>5.7</v>
       </c>
-      <c r="E3" s="7">
+      <c r="G3" s="8">
         <v>4.617</v>
       </c>
-      <c r="F3" s="8">
+      <c r="H3" s="9">
         <v>1.25</v>
       </c>
-      <c r="G3" s="8">
+      <c r="I3" s="9">
         <v>0.27</v>
       </c>
     </row>
-    <row r="4" ht="15.75" spans="1:7">
+    <row r="4" ht="15.75" spans="1:9">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4" s="5">
+        <v>177853.5</v>
+      </c>
+      <c r="D4" s="6">
+        <v>145516.5</v>
+      </c>
+      <c r="E4" s="6">
         <v>323370</v>
       </c>
-      <c r="D4" s="6">
+      <c r="F4" s="7">
         <v>10.05</v>
       </c>
-      <c r="E4" s="7">
+      <c r="G4" s="8">
         <v>7.638</v>
       </c>
-      <c r="F4" s="8">
+      <c r="H4" s="9">
         <v>1.34</v>
       </c>
-      <c r="G4" s="8">
+      <c r="I4" s="9">
         <v>0.33</v>
       </c>
     </row>
-    <row r="5" ht="15.75" spans="1:7">
+    <row r="5" ht="15.75" spans="1:9">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C5" s="5">
+        <v>198002.75</v>
+      </c>
+      <c r="D5" s="6">
+        <v>162002.25</v>
+      </c>
+      <c r="E5" s="6">
         <v>360005</v>
       </c>
-      <c r="D5" s="6">
+      <c r="F5" s="7">
         <v>4.56</v>
       </c>
-      <c r="E5" s="7">
+      <c r="G5" s="8">
         <v>3.8304</v>
       </c>
-      <c r="F5" s="8">
+      <c r="H5" s="9">
         <v>1.27</v>
       </c>
-      <c r="G5" s="8">
+      <c r="I5" s="9">
         <v>0.26</v>
       </c>
     </row>
-    <row r="6" ht="15.75" spans="1:7">
+    <row r="6" ht="15.75" spans="1:9">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C6" s="5">
+        <v>181663.9</v>
+      </c>
+      <c r="D6" s="6">
+        <v>148634.1</v>
+      </c>
+      <c r="E6" s="6">
         <v>330298</v>
       </c>
-      <c r="D6" s="6">
+      <c r="F6" s="7">
         <v>14.93</v>
       </c>
-      <c r="E6" s="7">
+      <c r="G6" s="8">
         <v>9.5552</v>
       </c>
-      <c r="F6" s="8">
+      <c r="H6" s="9">
         <v>1.31</v>
       </c>
-      <c r="G6" s="8">
+      <c r="I6" s="9">
         <v>0.24</v>
       </c>
     </row>
-    <row r="7" ht="15.75" spans="1:7">
+    <row r="7" ht="15.75" spans="1:9">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C7" s="5">
+        <v>199375</v>
+      </c>
+      <c r="D7" s="6">
+        <v>163125</v>
+      </c>
+      <c r="E7" s="6">
         <v>362500</v>
       </c>
-      <c r="D7" s="6">
+      <c r="F7" s="7">
         <v>6.32</v>
       </c>
-      <c r="E7" s="7">
+      <c r="G7" s="8">
         <v>5.372</v>
       </c>
-      <c r="F7" s="8">
+      <c r="H7" s="9">
         <v>1.29</v>
       </c>
-      <c r="G7" s="8">
+      <c r="I7" s="9">
         <v>0.25</v>
       </c>
     </row>
-    <row r="8" ht="15.75" spans="1:7">
+    <row r="8" ht="15.75" spans="1:9">
       <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C8" s="5">
+        <v>204733.1</v>
+      </c>
+      <c r="D8" s="6">
+        <v>167508.9</v>
+      </c>
+      <c r="E8" s="6">
         <v>372242</v>
       </c>
-      <c r="D8" s="6">
+      <c r="F8" s="7">
         <v>4.89</v>
       </c>
-      <c r="E8" s="7">
+      <c r="G8" s="8">
         <v>4.2543</v>
       </c>
-      <c r="F8" s="8">
+      <c r="H8" s="9">
         <v>1.25</v>
       </c>
-      <c r="G8" s="8">
+      <c r="I8" s="9">
         <v>0.26</v>
       </c>
     </row>
-    <row r="9" ht="15.75" spans="1:8">
+    <row r="9" ht="15.75" spans="1:10">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C9" s="5">
+        <v>205969.5</v>
+      </c>
+      <c r="D9" s="6">
+        <v>168520.5</v>
+      </c>
+      <c r="E9" s="6">
         <v>374490</v>
       </c>
-      <c r="D9" s="6">
+      <c r="F9" s="7">
         <v>6.71</v>
       </c>
-      <c r="E9" s="7">
+      <c r="G9" s="8">
         <v>5.7706</v>
       </c>
-      <c r="F9" s="8">
+      <c r="H9" s="9">
         <v>1.27</v>
       </c>
-      <c r="G9" s="8">
+      <c r="I9" s="9">
         <v>0.33</v>
       </c>
-      <c r="H9" s="9"/>
-    </row>
-    <row r="10" ht="15.75" spans="1:8">
+      <c r="J9" s="18"/>
+    </row>
+    <row r="10" ht="15.75" spans="1:10">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C10" s="5">
+        <v>218370.9</v>
+      </c>
+      <c r="D10" s="6">
+        <v>178667.1</v>
+      </c>
+      <c r="E10" s="6">
         <v>397038</v>
       </c>
-      <c r="D10" s="6">
+      <c r="F10" s="7">
         <v>5.08</v>
       </c>
-      <c r="E10" s="7">
+      <c r="G10" s="8">
         <v>4.318</v>
       </c>
-      <c r="F10" s="8">
+      <c r="H10" s="9">
         <v>1.29</v>
       </c>
-      <c r="G10" s="8">
+      <c r="I10" s="9">
         <v>0.23</v>
       </c>
-      <c r="H10" s="9"/>
-    </row>
-    <row r="11" ht="15.75" spans="1:7">
+      <c r="J10" s="18"/>
+    </row>
+    <row r="11" ht="15.75" spans="1:9">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C11" s="5">
+        <v>179207.05</v>
+      </c>
+      <c r="D11" s="6">
+        <v>146623.95</v>
+      </c>
+      <c r="E11" s="6">
         <v>325831</v>
       </c>
-      <c r="D11" s="6">
+      <c r="F11" s="7">
         <v>9.02</v>
       </c>
-      <c r="E11" s="7">
+      <c r="G11" s="8">
         <v>6.5846</v>
       </c>
-      <c r="F11" s="8">
+      <c r="H11" s="9">
         <v>1.33</v>
       </c>
-      <c r="G11" s="8">
+      <c r="I11" s="9">
         <v>0.31</v>
       </c>
     </row>
-    <row r="12" ht="15.75" spans="1:7">
+    <row r="12" ht="15.75" spans="1:9">
       <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C12" s="5">
+        <v>184562.95</v>
+      </c>
+      <c r="D12" s="6">
+        <v>151006.05</v>
+      </c>
+      <c r="E12" s="6">
         <v>335569</v>
       </c>
-      <c r="D12" s="6">
+      <c r="F12" s="7">
         <v>9.33</v>
       </c>
-      <c r="E12" s="7">
+      <c r="G12" s="8">
         <v>7.0908</v>
       </c>
-      <c r="F12" s="8">
+      <c r="H12" s="9">
         <v>1.31</v>
       </c>
-      <c r="G12" s="8">
+      <c r="I12" s="9">
         <v>0.26</v>
       </c>
     </row>
-    <row r="13" ht="15.75" spans="1:7">
+    <row r="13" ht="15.75" spans="1:9">
       <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C13" s="5">
+        <v>191448.4</v>
+      </c>
+      <c r="D13" s="6">
+        <v>156639.6</v>
+      </c>
+      <c r="E13" s="6">
         <v>348088</v>
       </c>
-      <c r="D13" s="6">
+      <c r="F13" s="7">
         <v>9.47</v>
       </c>
-      <c r="E13" s="7">
+      <c r="G13" s="8">
         <v>7.0078</v>
       </c>
-      <c r="F13" s="8">
+      <c r="H13" s="9">
         <v>1.32</v>
       </c>
-      <c r="G13" s="8">
+      <c r="I13" s="9">
         <v>0.3</v>
       </c>
     </row>
-    <row r="14" ht="15.75" spans="1:7">
+    <row r="14" ht="15.75" spans="1:9">
       <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C14" s="5">
+        <v>202324.1</v>
+      </c>
+      <c r="D14" s="6">
+        <v>165537.9</v>
+      </c>
+      <c r="E14" s="6">
         <v>367862</v>
       </c>
-      <c r="D14" s="6">
+      <c r="F14" s="7">
         <v>5.09</v>
       </c>
-      <c r="E14" s="7">
+      <c r="G14" s="8">
         <v>4.2247</v>
       </c>
-      <c r="F14" s="8">
+      <c r="H14" s="9">
         <v>1.29</v>
       </c>
-      <c r="G14" s="8">
+      <c r="I14" s="9">
         <v>0.24</v>
       </c>
     </row>
-    <row r="15" ht="15.75" spans="1:7">
+    <row r="15" ht="15.75" spans="1:9">
       <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C15" s="5">
+        <v>177381.6</v>
+      </c>
+      <c r="D15" s="6">
+        <v>145130.4</v>
+      </c>
+      <c r="E15" s="6">
         <v>322512</v>
       </c>
-      <c r="D15" s="6">
+      <c r="F15" s="7">
         <v>10.7</v>
       </c>
-      <c r="E15" s="7">
+      <c r="G15" s="8">
         <v>7.169</v>
       </c>
-      <c r="F15" s="8">
+      <c r="H15" s="9">
         <v>1.31</v>
       </c>
-      <c r="G15" s="8">
+      <c r="I15" s="9">
         <v>0.23</v>
       </c>
     </row>
-    <row r="16" ht="15.75" spans="1:7">
+    <row r="16" ht="15.75" spans="1:9">
       <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C16" s="5">
+        <v>208284.45</v>
+      </c>
+      <c r="D16" s="6">
+        <v>170414.55</v>
+      </c>
+      <c r="E16" s="6">
         <v>378699</v>
       </c>
-      <c r="D16" s="6">
+      <c r="F16" s="7">
         <v>7.64</v>
       </c>
-      <c r="E16" s="7">
+      <c r="G16" s="8">
         <v>5.8828</v>
       </c>
-      <c r="F16" s="8">
+      <c r="H16" s="9">
         <v>1.25</v>
       </c>
-      <c r="G16" s="8">
+      <c r="I16" s="9">
         <v>0.32</v>
       </c>
     </row>
-    <row r="17" ht="15.75" spans="1:7">
+    <row r="17" ht="15.75" spans="1:9">
       <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C17" s="5">
+        <v>226779.85</v>
+      </c>
+      <c r="D17" s="6">
+        <v>185547.15</v>
+      </c>
+      <c r="E17" s="6">
         <v>412327</v>
       </c>
-      <c r="D17" s="6">
+      <c r="F17" s="7">
         <v>7.37</v>
       </c>
-      <c r="E17" s="7">
+      <c r="G17" s="8">
         <v>5.5275</v>
       </c>
-      <c r="F17" s="8">
+      <c r="H17" s="9">
         <v>1.26</v>
       </c>
-      <c r="G17" s="8">
+      <c r="I17" s="9">
         <v>0.24</v>
       </c>
     </row>
-    <row r="18" ht="15.75" spans="1:7">
+    <row r="18" ht="15.75" spans="1:9">
       <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C18" s="5">
+        <v>223121.8</v>
+      </c>
+      <c r="D18" s="6">
+        <v>182554.2</v>
+      </c>
+      <c r="E18" s="6">
         <v>405676</v>
       </c>
-      <c r="D18" s="6">
+      <c r="F18" s="7">
         <v>4.65</v>
       </c>
-      <c r="E18" s="7">
+      <c r="G18" s="8">
         <v>4.092</v>
       </c>
-      <c r="F18" s="8">
+      <c r="H18" s="9">
         <v>1.25</v>
       </c>
-      <c r="G18" s="8">
+      <c r="I18" s="9">
         <v>0.25</v>
       </c>
     </row>
-    <row r="19" ht="15.75" spans="1:7">
+    <row r="19" ht="15.75" spans="1:9">
       <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C19" s="5">
+        <v>176689.7</v>
+      </c>
+      <c r="D19" s="6">
+        <v>144564.3</v>
+      </c>
+      <c r="E19" s="6">
         <v>321254</v>
       </c>
-      <c r="D19" s="6">
+      <c r="F19" s="7">
         <v>7.31</v>
       </c>
-      <c r="E19" s="7">
+      <c r="G19" s="8">
         <v>5.4094</v>
       </c>
-      <c r="F19" s="8">
+      <c r="H19" s="9">
         <v>1.32</v>
       </c>
-      <c r="G19" s="8">
+      <c r="I19" s="9">
         <v>0.3</v>
       </c>
     </row>
-    <row r="20" ht="15.75" spans="1:7">
+    <row r="20" ht="15.75" spans="1:9">
       <c r="A20" s="3">
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C20" s="5">
+        <v>190952.3</v>
+      </c>
+      <c r="D20" s="6">
+        <v>156233.7</v>
+      </c>
+      <c r="E20" s="6">
         <v>347186</v>
       </c>
-      <c r="D20" s="6">
+      <c r="F20" s="7">
         <v>7.78</v>
       </c>
-      <c r="E20" s="7">
+      <c r="G20" s="8">
         <v>5.6016</v>
       </c>
-      <c r="F20" s="8">
+      <c r="H20" s="9">
         <v>1.26</v>
       </c>
-      <c r="G20" s="8">
+      <c r="I20" s="9">
         <v>0.32</v>
       </c>
     </row>
-    <row r="21" ht="15.75" spans="1:7">
+    <row r="21" ht="15.75" spans="1:9">
       <c r="A21" s="3">
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C21" s="5">
+        <v>187017.05</v>
+      </c>
+      <c r="D21" s="6">
+        <v>153013.95</v>
+      </c>
+      <c r="E21" s="6">
         <v>340031</v>
       </c>
-      <c r="D21" s="6">
+      <c r="F21" s="7">
         <v>13.16</v>
       </c>
-      <c r="E21" s="7">
+      <c r="G21" s="8">
         <v>8.6856</v>
       </c>
-      <c r="F21" s="8">
+      <c r="H21" s="9">
         <v>1.31</v>
       </c>
-      <c r="G21" s="8">
+      <c r="I21" s="9">
         <v>0.28</v>
       </c>
     </row>
-    <row r="22" ht="15.75" spans="1:7">
+    <row r="22" ht="15.75" spans="1:9">
       <c r="A22" s="3">
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C22" s="5">
+        <v>199124.75</v>
+      </c>
+      <c r="D22" s="6">
+        <v>162920.25</v>
+      </c>
+      <c r="E22" s="6">
         <v>362045</v>
       </c>
-      <c r="D22" s="6">
+      <c r="F22" s="7">
         <v>6.15</v>
       </c>
-      <c r="E22" s="7">
+      <c r="G22" s="8">
         <v>4.9815</v>
       </c>
-      <c r="F22" s="8">
+      <c r="H22" s="9">
         <v>1.34</v>
       </c>
-      <c r="G22" s="8">
+      <c r="I22" s="9">
         <v>0.27</v>
       </c>
     </row>
-    <row r="23" ht="15.75" spans="1:7">
+    <row r="23" ht="15.75" spans="1:9">
       <c r="A23" s="3">
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C23" s="5">
+        <v>209584.65</v>
+      </c>
+      <c r="D23" s="6">
+        <v>171478.35</v>
+      </c>
+      <c r="E23" s="6">
         <v>381063</v>
       </c>
-      <c r="D23" s="6">
+      <c r="F23" s="7">
         <v>6.05</v>
       </c>
-      <c r="E23" s="7">
+      <c r="G23" s="8">
         <v>5.0215</v>
       </c>
-      <c r="F23" s="8">
+      <c r="H23" s="9">
         <v>1.3</v>
       </c>
-      <c r="G23" s="8">
+      <c r="I23" s="9">
         <v>0.29</v>
       </c>
     </row>
-    <row r="24" ht="15.75" spans="1:7">
+    <row r="24" ht="15.75" spans="1:9">
       <c r="A24" s="3">
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C24" s="5">
+        <v>183119.2</v>
+      </c>
+      <c r="D24" s="6">
+        <v>149824.8</v>
+      </c>
+      <c r="E24" s="6">
         <v>332944</v>
       </c>
-      <c r="D24" s="6">
+      <c r="F24" s="7">
         <v>10.12</v>
       </c>
-      <c r="E24" s="7">
+      <c r="G24" s="8">
         <v>7.1852</v>
       </c>
-      <c r="F24" s="8">
+      <c r="H24" s="9">
         <v>1.25</v>
       </c>
-      <c r="G24" s="8">
+      <c r="I24" s="9">
         <v>0.25</v>
       </c>
     </row>
-    <row r="25" ht="15.75" spans="1:7">
+    <row r="25" ht="15.75" spans="1:9">
       <c r="A25" s="3">
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C25" s="5">
+        <v>211433.75</v>
+      </c>
+      <c r="D25" s="6">
+        <v>172991.25</v>
+      </c>
+      <c r="E25" s="6">
         <v>384425</v>
       </c>
-      <c r="D25" s="6">
+      <c r="F25" s="7">
         <v>8.83</v>
       </c>
-      <c r="E25" s="7">
+      <c r="G25" s="8">
         <v>6.7108</v>
       </c>
-      <c r="F25" s="8">
+      <c r="H25" s="9">
         <v>1.32</v>
       </c>
-      <c r="G25" s="8">
+      <c r="I25" s="9">
         <v>0.23</v>
       </c>
     </row>
-    <row r="26" ht="15.75" spans="1:7">
+    <row r="26" ht="15.75" spans="1:9">
       <c r="A26" s="10">
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C26" s="5">
+        <v>190472.7</v>
+      </c>
+      <c r="D26" s="6">
+        <v>155841.3</v>
+      </c>
+      <c r="E26" s="6">
         <v>346314</v>
       </c>
-      <c r="D26" s="6">
+      <c r="F26" s="7">
         <v>7.69</v>
       </c>
-      <c r="E26" s="7">
+      <c r="G26" s="8">
         <v>6.2289</v>
       </c>
-      <c r="F26" s="8">
+      <c r="H26" s="9">
         <v>1.29</v>
       </c>
-      <c r="G26" s="8">
+      <c r="I26" s="9">
         <v>0.31</v>
       </c>
     </row>
-    <row r="27" ht="15.75" spans="1:7">
+    <row r="27" ht="15.75" spans="1:9">
       <c r="A27" s="11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C27" s="13">
+        <v>212801.05</v>
+      </c>
+      <c r="D27" s="14">
+        <v>174109.95</v>
+      </c>
+      <c r="E27" s="14">
         <v>386911</v>
       </c>
-      <c r="D27" s="14">
+      <c r="F27" s="15">
         <v>8.07</v>
       </c>
-      <c r="E27" s="15">
+      <c r="G27" s="16">
         <v>6.3753</v>
       </c>
-      <c r="F27" s="16">
+      <c r="H27" s="17">
         <v>1.31</v>
       </c>
-      <c r="G27" s="16">
+      <c r="I27" s="17">
         <v>0.29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revisi Rekap Excel Kemiskinan Tambah Gini Rasio
</commit_message>
<xml_diff>
--- a/Rekap/RekapKemiskinan.xlsx
+++ b/Rekap/RekapKemiskinan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>No</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>Indeks Keparahan Kemiskinan</t>
+  </si>
+  <si>
+    <t>Gini Rasio</t>
   </si>
   <si>
     <t>Pesanggaran</t>
@@ -129,14 +132,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="&quot;Rp&quot;#,##0_);[Red]\(&quot;Rp&quot;#,##0\)"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="0.00_ "/>
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
+    <numFmt numFmtId="177" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="180" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="180" formatCode="&quot;Rp&quot;#,##0_);[Red]\(&quot;Rp&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,11 +176,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Consolas"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -188,6 +186,113 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -199,98 +304,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -300,22 +313,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -336,6 +334,150 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -348,13 +490,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -366,151 +508,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -552,36 +550,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -593,24 +561,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -633,8 +583,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -649,153 +614,186 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -809,19 +807,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="1" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -833,23 +831,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1185,7 +1186,7 @@
     <col min="6" max="9" width="12.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="47.25" customHeight="1" spans="1:9">
+    <row r="1" ht="47.25" customHeight="1" spans="1:10">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1213,13 +1214,16 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" ht="15.75" spans="1:9">
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" ht="15.75" spans="1:10">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="5">
         <v>177141.8</v>
@@ -1242,13 +1246,16 @@
       <c r="I2" s="9">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="3" ht="15.75" spans="1:9">
+      <c r="J2" s="18">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="3" ht="15.75" spans="1:10">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="5">
         <v>200626.8</v>
@@ -1271,13 +1278,16 @@
       <c r="I3" s="9">
         <v>0.27</v>
       </c>
-    </row>
-    <row r="4" ht="15.75" spans="1:9">
+      <c r="J3" s="18">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="4" ht="15.75" spans="1:10">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="5">
         <v>177853.5</v>
@@ -1300,13 +1310,16 @@
       <c r="I4" s="9">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="5" ht="15.75" spans="1:9">
+      <c r="J4" s="18">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="5" ht="15.75" spans="1:10">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="5">
         <v>198002.75</v>
@@ -1329,13 +1342,16 @@
       <c r="I5" s="9">
         <v>0.26</v>
       </c>
-    </row>
-    <row r="6" ht="15.75" spans="1:9">
+      <c r="J5" s="18">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="6" ht="15.75" spans="1:10">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="5">
         <v>181663.9</v>
@@ -1358,13 +1374,16 @@
       <c r="I6" s="9">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="7" ht="15.75" spans="1:9">
+      <c r="J6" s="18">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="7" ht="15.75" spans="1:10">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" s="5">
         <v>199375</v>
@@ -1387,13 +1406,16 @@
       <c r="I7" s="9">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="8" ht="15.75" spans="1:9">
+      <c r="J7" s="18">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="8" ht="15.75" spans="1:10">
       <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8" s="5">
         <v>204733.1</v>
@@ -1415,6 +1437,9 @@
       </c>
       <c r="I8" s="9">
         <v>0.26</v>
+      </c>
+      <c r="J8" s="18">
+        <v>0.33</v>
       </c>
     </row>
     <row r="9" ht="15.75" spans="1:10">
@@ -1422,7 +1447,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C9" s="5">
         <v>205969.5</v>
@@ -1445,14 +1470,16 @@
       <c r="I9" s="9">
         <v>0.33</v>
       </c>
-      <c r="J9" s="18"/>
+      <c r="J9" s="18">
+        <v>0.42</v>
+      </c>
     </row>
     <row r="10" ht="15.75" spans="1:10">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" s="5">
         <v>218370.9</v>
@@ -1475,14 +1502,16 @@
       <c r="I10" s="9">
         <v>0.23</v>
       </c>
-      <c r="J10" s="18"/>
-    </row>
-    <row r="11" ht="15.75" spans="1:9">
+      <c r="J10" s="18">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="11" ht="15.75" spans="1:10">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C11" s="5">
         <v>179207.05</v>
@@ -1505,13 +1534,16 @@
       <c r="I11" s="9">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="12" ht="15.75" spans="1:9">
+      <c r="J11" s="18">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="12" ht="15.75" spans="1:10">
       <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C12" s="5">
         <v>184562.95</v>
@@ -1534,13 +1566,16 @@
       <c r="I12" s="9">
         <v>0.26</v>
       </c>
-    </row>
-    <row r="13" ht="15.75" spans="1:9">
+      <c r="J12" s="18">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="13" ht="15.75" spans="1:10">
       <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C13" s="5">
         <v>191448.4</v>
@@ -1563,13 +1598,16 @@
       <c r="I13" s="9">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="14" ht="15.75" spans="1:9">
+      <c r="J13" s="18">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="14" ht="15.75" spans="1:10">
       <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C14" s="5">
         <v>202324.1</v>
@@ -1592,13 +1630,16 @@
       <c r="I14" s="9">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="15" ht="15.75" spans="1:9">
+      <c r="J14" s="18">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="15" ht="15.75" spans="1:10">
       <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C15" s="5">
         <v>177381.6</v>
@@ -1621,13 +1662,16 @@
       <c r="I15" s="9">
         <v>0.23</v>
       </c>
-    </row>
-    <row r="16" ht="15.75" spans="1:9">
+      <c r="J15" s="18">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="16" ht="15.75" spans="1:10">
       <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C16" s="5">
         <v>208284.45</v>
@@ -1650,13 +1694,16 @@
       <c r="I16" s="9">
         <v>0.32</v>
       </c>
-    </row>
-    <row r="17" ht="15.75" spans="1:9">
+      <c r="J16" s="18">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="17" ht="15.75" spans="1:10">
       <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C17" s="5">
         <v>226779.85</v>
@@ -1679,13 +1726,16 @@
       <c r="I17" s="9">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="18" ht="15.75" spans="1:9">
+      <c r="J17" s="18">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="18" ht="15.75" spans="1:10">
       <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C18" s="5">
         <v>223121.8</v>
@@ -1708,13 +1758,16 @@
       <c r="I18" s="9">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="19" ht="15.75" spans="1:9">
+      <c r="J18" s="18">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="19" ht="15.75" spans="1:10">
       <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C19" s="5">
         <v>176689.7</v>
@@ -1737,13 +1790,16 @@
       <c r="I19" s="9">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="20" ht="15.75" spans="1:9">
+      <c r="J19" s="18">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="20" ht="15.75" spans="1:10">
       <c r="A20" s="3">
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C20" s="5">
         <v>190952.3</v>
@@ -1766,13 +1822,16 @@
       <c r="I20" s="9">
         <v>0.32</v>
       </c>
-    </row>
-    <row r="21" ht="15.75" spans="1:9">
+      <c r="J20" s="18">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="21" ht="15.75" spans="1:10">
       <c r="A21" s="3">
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C21" s="5">
         <v>187017.05</v>
@@ -1795,13 +1854,16 @@
       <c r="I21" s="9">
         <v>0.28</v>
       </c>
-    </row>
-    <row r="22" ht="15.75" spans="1:9">
+      <c r="J21" s="18">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="22" ht="15.75" spans="1:10">
       <c r="A22" s="3">
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C22" s="5">
         <v>199124.75</v>
@@ -1824,13 +1886,16 @@
       <c r="I22" s="9">
         <v>0.27</v>
       </c>
-    </row>
-    <row r="23" ht="15.75" spans="1:9">
+      <c r="J22" s="18">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="23" ht="15.75" spans="1:10">
       <c r="A23" s="3">
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C23" s="5">
         <v>209584.65</v>
@@ -1853,13 +1918,16 @@
       <c r="I23" s="9">
         <v>0.29</v>
       </c>
-    </row>
-    <row r="24" ht="15.75" spans="1:9">
+      <c r="J23" s="18">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="24" ht="15.75" spans="1:10">
       <c r="A24" s="3">
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C24" s="5">
         <v>183119.2</v>
@@ -1882,13 +1950,16 @@
       <c r="I24" s="9">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="25" ht="15.75" spans="1:9">
+      <c r="J24" s="18">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="25" ht="15.75" spans="1:10">
       <c r="A25" s="3">
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C25" s="5">
         <v>211433.75</v>
@@ -1911,13 +1982,16 @@
       <c r="I25" s="9">
         <v>0.23</v>
       </c>
-    </row>
-    <row r="26" ht="15.75" spans="1:9">
+      <c r="J25" s="18">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="26" ht="15.75" spans="1:10">
       <c r="A26" s="10">
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C26" s="5">
         <v>190472.7</v>
@@ -1940,13 +2014,16 @@
       <c r="I26" s="9">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="27" ht="15.75" spans="1:9">
+      <c r="J26" s="18">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="27" ht="15.75" spans="1:10">
       <c r="A27" s="11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C27" s="13">
         <v>212801.05</v>
@@ -1968,6 +2045,9 @@
       </c>
       <c r="I27" s="17">
         <v>0.29</v>
+      </c>
+      <c r="J27" s="19">
+        <v>0.36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>